<commit_message>
Fixed issue related to the extraction of data from table
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\UIPathLearning\TableExtractionFromACME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CA99D3-4BC2-4D8D-A153-9B6B782FC230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C839802B-218B-406A-8084-4A8A687D337B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="14">
   <si>
     <t>WIID</t>
   </si>
@@ -102,8 +103,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -385,11 +392,978 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>106485094</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>106485155</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>106485177</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>43656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>106485169</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>106485101</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>106485161</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42849</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>106485113</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>106485150</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>43480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>106485100</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>106485147</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>106485094</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>106485155</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>106485177</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>43656</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>106485169</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>106485101</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>106485161</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2">
+        <v>42849</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>106485113</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>106485150</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2">
+        <v>43480</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>106485100</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>106485147</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2">
+        <v>45163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>106485094</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>106485155</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="2">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>106485177</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2">
+        <v>43656</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>106485169</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>106485101</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2">
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>106485161</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="2">
+        <v>42849</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>106485113</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>106485150</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="2">
+        <v>43480</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>106485100</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>106485147</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2">
+        <v>45163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>106485094</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="2">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>106485155</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="2">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>106485177</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="2">
+        <v>43656</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>106485169</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="2">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>106485101</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="2">
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>106485161</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="2">
+        <v>42849</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>106485113</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="2">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>106485150</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="2">
+        <v>43480</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>106485100</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="2">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>106485147</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>106485094</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="2">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>106485155</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="2">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>106485177</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="2">
+        <v>43656</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>106485169</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="2">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>106485101</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2">
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>106485161</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="2">
+        <v>42849</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>106485113</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="2">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>106485150</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="2">
+        <v>43480</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>106485100</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="2">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>106485147</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="2">
+        <v>45163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1325B5-A6D2-4F4C-A9EA-BCC9A6E89BCE}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -421,7 +1395,7 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>42870</v>
       </c>
     </row>
@@ -438,7 +1412,7 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>45013</v>
       </c>
     </row>
@@ -455,7 +1429,7 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>43656</v>
       </c>
     </row>
@@ -472,7 +1446,7 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>45261</v>
       </c>
     </row>
@@ -489,7 +1463,7 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <v>45434</v>
       </c>
     </row>
@@ -506,7 +1480,7 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <v>42849</v>
       </c>
     </row>
@@ -523,7 +1497,7 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>43732</v>
       </c>
     </row>
@@ -540,7 +1514,7 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>43480</v>
       </c>
     </row>
@@ -557,7 +1531,7 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>42852</v>
       </c>
     </row>
@@ -574,7 +1548,7 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>45163</v>
       </c>
     </row>

</xml_diff>